<commit_message>
declared drivers path as constants
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testData/TestDocument.xlsx
+++ b/src/main/java/com/qa/testData/TestDocument.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5891616F-4AA5-4FD5-ABD8-FC59FE034805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4185713-CB0D-4AC1-AC10-F7A41C7AA8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Cookie" sheetId="3" r:id="rId3"/>
-    <sheet name="TestScripts" sheetId="5" r:id="rId4"/>
+    <sheet name="Cookie" sheetId="3" r:id="rId2"/>
+    <sheet name="TestScripts" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Deepak</t>
   </si>
@@ -113,18 +112,6 @@
   </si>
   <si>
     <t>GA1.2.1256884372.1538366534</t>
-  </si>
-  <si>
-    <t>AdressData1</t>
-  </si>
-  <si>
-    <t>Address2</t>
-  </si>
-  <si>
-    <t>Row House No 5</t>
-  </si>
-  <si>
-    <t>Gajanana Society</t>
   </si>
   <si>
     <t>TestName</t>
@@ -505,7 +492,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,46 +566,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107D4962-AC65-438D-8689-9A16F1ED8D86}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06492BDE-2B4B-4F89-BB75-8F1820AD6273}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,12 +699,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEEB11A-B40C-46D4-A57F-2FFDDA4EBE53}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,15 +715,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>

</xml_diff>